<commit_message>
Przyjmijmy, że DB jest zasilona w schemat
</commit_message>
<xml_diff>
--- a/doc/template.xlsx
+++ b/doc/template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -2130,10 +2130,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2165,10 +2165,6 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>